<commit_message>
Add support for importing the new fields via uploads
</commit_message>
<xml_diff>
--- a/digital_agenda/apps/core/static/import_file_example.xlsx
+++ b/digital_agenda/apps/core/static/import_file_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">period</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference_period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarks</t>
   </si>
   <si>
     <t xml:space="preserve">EU</t>
@@ -67,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,8 +133,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,54 +159,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>17.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add reference period and remarks fields for facts  (#102)
* Rename existing remarks field

In preparation for adding the remark dimension field

* Add new fields for fact and populate them from extra notes

* Add support for importing the new fields via uploads

* Add tests for new field uploads and XLS uplods

* Add the ability to import the two new fields from ESTAT

* Add tests for ESTAT imports of the new fields

* Include the new fields in the API and exports

* Include remarks in the tooltips

* Don't migrate extra chart notes automatically

Use a management command instead

* Include reference period in the tooltip
</commit_message>
<xml_diff>
--- a/digital_agenda/apps/core/static/import_file_example.xlsx
+++ b/digital_agenda/apps/core/static/import_file_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">period</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference_period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarks</t>
   </si>
   <si>
     <t xml:space="preserve">EU</t>
@@ -67,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,8 +133,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,54 +159,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>17.6</v>
       </c>
     </row>

</xml_diff>